<commit_message>
Learned Classes and Objects, updated Log Book
</commit_message>
<xml_diff>
--- a/DSA LogBook.xlsx
+++ b/DSA LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akshi\DSA_Restart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE7A627-BC51-44CE-BE21-D02B27F546AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727AF550-33D8-4309-A06A-6A211FEC7192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2EBF366D-E6C4-46CB-805E-4E078FCDBBBC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Leetcode problems</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Bit-Manipulation (Concepts)</t>
+  </si>
+  <si>
+    <t>Bit Manipulation Questions</t>
+  </si>
+  <si>
+    <t>100 mins</t>
+  </si>
+  <si>
+    <t>Compled bit-manipulation and started OOP concepts</t>
+  </si>
+  <si>
+    <t>count bits - 338</t>
+  </si>
+  <si>
+    <t>150-180 mins</t>
   </si>
 </sst>
 </file>
@@ -484,7 +499,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,11 +634,33 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="3"/>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>46073</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="3"/>

</xml_diff>